<commit_message>
Worked on standard naming convention documentation in "Wings_3D_Library_Info.xlsx", "KiCAD_PCB_Library_Info.xlsx" documents
Added feature requests to "KiCAD Feature Requests.rtf" document

Added following components to Passive PCB Library
 - RES_M_500MIL_375MIL_195MIL_HORZ_PTH
 - RES_M_500MIL_375MIL_195MIL_PTH

Changed footprint association for the Electromechanical Schematic Library
component, FSMJH, from 3D Component "SW_TACT_PUSH" to "FSMJH" to lock it to that
specific footprint.

Added several 3D Component Potentiometer Library components to repo using. These
components were part of the KiCAD package and were renamed using the standard
naming convention.
</commit_message>
<xml_diff>
--- a/3D/Wings_3D_Library_Info.xlsx
+++ b/3D/Wings_3D_Library_Info.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="270" yWindow="570" windowWidth="20775" windowHeight="10425" activeTab="2"/>
+    <workbookView xWindow="270" yWindow="570" windowWidth="20775" windowHeight="10425" tabRatio="719" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Library Names" sheetId="1" r:id="rId1"/>
@@ -23,12 +23,11 @@
     <sheet name="Test" sheetId="14" r:id="rId14"/>
   </sheets>
   <calcPr calcId="0"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2063" uniqueCount="537">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2065" uniqueCount="539">
   <si>
     <t>Battery</t>
   </si>
@@ -1639,6 +1638,12 @@
   </si>
   <si>
     <t>CONNECTOR_USB_TYPE_B_M_RA_PTH</t>
+  </si>
+  <si>
+    <t>RES_500_375D_195L_HORZ_PTH</t>
+  </si>
+  <si>
+    <t>RES_M_500MIL_375MIL_195MIL_HORZ_PTH</t>
   </si>
 </sst>
 </file>
@@ -1725,18 +1730,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Heading" xfId="1"/>
@@ -2138,7 +2143,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11.625" style="3" customWidth="1"/>
     <col min="2" max="2" width="13.625" style="3" customWidth="1"/>
@@ -2156,11 +2161,11 @@
       <c r="C1" s="2" t="s">
         <v>414</v>
       </c>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-    </row>
-    <row r="2" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>415</v>
       </c>
@@ -2171,7 +2176,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>417</v>
       </c>
@@ -2182,7 +2187,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>418</v>
       </c>
@@ -2193,7 +2198,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>419</v>
       </c>
@@ -2204,7 +2209,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>420</v>
       </c>
@@ -2215,7 +2220,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>421</v>
       </c>
@@ -2226,7 +2231,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>422</v>
       </c>
@@ -2237,7 +2242,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>423</v>
       </c>
@@ -2248,7 +2253,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>424</v>
       </c>
@@ -2259,7 +2264,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>426</v>
       </c>
@@ -2270,7 +2275,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>427</v>
       </c>
@@ -2281,7 +2286,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>428</v>
       </c>
@@ -2292,7 +2297,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>429</v>
       </c>
@@ -2303,7 +2308,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>430</v>
       </c>
@@ -2314,7 +2319,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>431</v>
       </c>
@@ -2325,7 +2330,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>432</v>
       </c>
@@ -2336,7 +2341,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>433</v>
       </c>
@@ -2347,7 +2352,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
         <v>434</v>
       </c>
@@ -2358,7 +2363,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
         <v>436</v>
       </c>
@@ -2369,7 +2374,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
         <v>437</v>
       </c>
@@ -2380,7 +2385,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
         <v>439</v>
       </c>
@@ -2391,7 +2396,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
         <v>440</v>
       </c>
@@ -2402,7 +2407,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
         <v>441</v>
       </c>
@@ -2413,7 +2418,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
         <v>442</v>
       </c>
@@ -2424,7 +2429,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
         <v>443</v>
       </c>
@@ -2435,7 +2440,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
         <v>444</v>
       </c>
@@ -2446,7 +2451,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
         <v>445</v>
       </c>
@@ -2457,7 +2462,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
         <v>446</v>
       </c>
@@ -2468,7 +2473,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
         <v>447</v>
       </c>
@@ -2479,7 +2484,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
         <v>449</v>
       </c>
@@ -2490,7 +2495,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
         <v>450</v>
       </c>
@@ -2501,7 +2506,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
         <v>447</v>
       </c>
@@ -2512,7 +2517,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
         <v>449</v>
       </c>
@@ -2523,7 +2528,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
         <v>451</v>
       </c>
@@ -2534,7 +2539,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
         <v>452</v>
       </c>
@@ -2545,7 +2550,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
         <v>453</v>
       </c>
@@ -2556,7 +2561,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
         <v>454</v>
       </c>
@@ -2567,7 +2572,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
         <v>455</v>
       </c>
@@ -2578,7 +2583,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" s="3" t="s">
         <v>456</v>
       </c>
@@ -2589,7 +2594,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" s="3" t="s">
         <v>457</v>
       </c>
@@ -2600,7 +2605,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" s="3" t="s">
         <v>459</v>
       </c>
@@ -2611,7 +2616,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" s="3" t="s">
         <v>460</v>
       </c>
@@ -2622,7 +2627,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="44" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" s="3" t="s">
         <v>461</v>
       </c>
@@ -2633,7 +2638,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="45" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" s="3" t="s">
         <v>462</v>
       </c>
@@ -2644,7 +2649,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="46" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" s="3" t="s">
         <v>464</v>
       </c>
@@ -2655,7 +2660,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="47" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" s="3" t="s">
         <v>465</v>
       </c>
@@ -2666,7 +2671,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="48" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" s="3" t="s">
         <v>466</v>
       </c>
@@ -2677,7 +2682,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="49" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" s="3" t="s">
         <v>467</v>
       </c>
@@ -2688,7 +2693,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="50" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" s="3" t="s">
         <v>468</v>
       </c>
@@ -2699,7 +2704,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="51" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" s="3" t="s">
         <v>469</v>
       </c>
@@ -2710,7 +2715,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="52" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" s="3" t="s">
         <v>470</v>
       </c>
@@ -2721,7 +2726,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="53" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" s="3" t="s">
         <v>471</v>
       </c>
@@ -2732,7 +2737,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="54" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" s="3" t="s">
         <v>472</v>
       </c>
@@ -2743,7 +2748,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="55" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" s="3" t="s">
         <v>474</v>
       </c>
@@ -2754,7 +2759,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="56" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" s="3" t="s">
         <v>475</v>
       </c>
@@ -2765,7 +2770,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="57" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57" s="3" t="s">
         <v>476</v>
       </c>
@@ -2776,7 +2781,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="58" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" s="3" t="s">
         <v>477</v>
       </c>
@@ -2787,7 +2792,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="59" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59" s="3" t="s">
         <v>478</v>
       </c>
@@ -2798,7 +2803,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="60" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" s="3" t="s">
         <v>479</v>
       </c>
@@ -2809,7 +2814,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="61" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61" s="3" t="s">
         <v>480</v>
       </c>
@@ -2820,7 +2825,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="62" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62" s="3" t="s">
         <v>481</v>
       </c>
@@ -2831,7 +2836,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="63" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A63" s="3" t="s">
         <v>482</v>
       </c>
@@ -2842,7 +2847,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="64" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A64" s="3" t="s">
         <v>484</v>
       </c>
@@ -2853,7 +2858,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="65" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65" s="3" t="s">
         <v>485</v>
       </c>
@@ -2864,7 +2869,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="66" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A66" s="3" t="s">
         <v>486</v>
       </c>
@@ -2875,7 +2880,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="67" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A67" s="3" t="s">
         <v>487</v>
       </c>
@@ -2886,7 +2891,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="68" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A68" s="3" t="s">
         <v>488</v>
       </c>
@@ -2897,7 +2902,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="69" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69" s="3" t="s">
         <v>489</v>
       </c>
@@ -2908,7 +2913,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="70" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A70" s="3" t="s">
         <v>490</v>
       </c>
@@ -2919,7 +2924,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="71" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A71" s="3" t="s">
         <v>491</v>
       </c>
@@ -2930,7 +2935,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="72" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A72" s="3" t="s">
         <v>492</v>
       </c>
@@ -2941,7 +2946,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="73" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A73" s="3" t="s">
         <v>493</v>
       </c>
@@ -2952,7 +2957,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="74" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A74" s="3" t="s">
         <v>494</v>
       </c>
@@ -2963,7 +2968,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="75" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A75" s="3" t="s">
         <v>495</v>
       </c>
@@ -2974,7 +2979,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="76" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A76" s="3" t="s">
         <v>497</v>
       </c>
@@ -2985,7 +2990,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="77" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A77" s="3" t="s">
         <v>498</v>
       </c>
@@ -2996,7 +3001,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="78" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A78" s="3" t="s">
         <v>499</v>
       </c>
@@ -3007,7 +3012,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="79" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A79" s="3" t="s">
         <v>500</v>
       </c>
@@ -3018,7 +3023,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="80" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A80" s="3" t="s">
         <v>501</v>
       </c>
@@ -3029,7 +3034,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="81" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A81" s="3" t="s">
         <v>502</v>
       </c>
@@ -3040,7 +3045,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="82" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A82" s="3" t="s">
         <v>503</v>
       </c>
@@ -3051,7 +3056,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="83" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A83" s="3" t="s">
         <v>504</v>
       </c>
@@ -3062,7 +3067,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="84" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A84" s="3" t="s">
         <v>506</v>
       </c>
@@ -3073,7 +3078,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="85" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A85" s="3" t="s">
         <v>507</v>
       </c>
@@ -3084,7 +3089,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="86" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A86" s="3" t="s">
         <v>508</v>
       </c>
@@ -3095,7 +3100,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="87" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A87" s="3" t="s">
         <v>509</v>
       </c>
@@ -3106,7 +3111,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="88" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A88" s="3" t="s">
         <v>510</v>
       </c>
@@ -3117,7 +3122,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="89" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A89" s="3" t="s">
         <v>511</v>
       </c>
@@ -3128,7 +3133,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="90" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A90" s="3" t="s">
         <v>512</v>
       </c>
@@ -3139,7 +3144,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="91" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A91" s="3" t="s">
         <v>513</v>
       </c>
@@ -3150,7 +3155,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="92" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A92" s="3" t="s">
         <v>514</v>
       </c>
@@ -3161,7 +3166,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="93" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A93" s="3" t="s">
         <v>515</v>
       </c>
@@ -3172,7 +3177,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="94" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A94" s="3" t="s">
         <v>516</v>
       </c>
@@ -3332,7 +3337,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
@@ -3345,7 +3350,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="7" t="s">
         <v>525</v>
       </c>
     </row>
@@ -3364,22 +3369,22 @@
       <c r="F2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4" t="s">
+      <c r="H2" s="8"/>
+      <c r="I2" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="J2" s="4"/>
-      <c r="K2" s="4" t="s">
+      <c r="J2" s="8"/>
+      <c r="K2" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="L2" s="4"/>
-      <c r="M2" s="4" t="s">
+      <c r="L2" s="8"/>
+      <c r="M2" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="N2" s="4"/>
+      <c r="N2" s="8"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
@@ -3458,7 +3463,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="29.125" customWidth="1"/>
     <col min="2" max="2" width="15.75" style="3" customWidth="1"/>
@@ -3484,44 +3489,44 @@
       <c r="F1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4" t="s">
+      <c r="H1" s="8"/>
+      <c r="I1" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4" t="s">
+      <c r="J1" s="8"/>
+      <c r="K1" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="L1" s="4"/>
-      <c r="M1" s="4" t="s">
+      <c r="L1" s="8"/>
+      <c r="M1" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="N1" s="4"/>
-    </row>
-    <row r="2" spans="1:14" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="N1" s="8"/>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>23</v>
       </c>
@@ -3562,7 +3567,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>29</v>
       </c>
@@ -3603,7 +3608,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>33</v>
       </c>
@@ -3647,7 +3652,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>37</v>
       </c>
@@ -3691,7 +3696,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>40</v>
       </c>
@@ -3749,17 +3754,18 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N10"/>
+  <dimension ref="A1:N13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="29.125" customWidth="1"/>
+    <col min="1" max="1" width="39" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.75" style="3" customWidth="1"/>
-    <col min="3" max="4" width="17.25" style="3" customWidth="1"/>
+    <col min="3" max="3" width="17.25" style="3" customWidth="1"/>
+    <col min="4" max="4" width="17.875" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.125" style="3" customWidth="1"/>
     <col min="6" max="6" width="13.75" style="3" customWidth="1"/>
     <col min="7" max="10" width="6" style="3" customWidth="1"/>
@@ -3781,44 +3787,44 @@
       <c r="F1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4" t="s">
+      <c r="H1" s="8"/>
+      <c r="I1" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4" t="s">
+      <c r="J1" s="8"/>
+      <c r="K1" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="L1" s="4"/>
-      <c r="M1" s="4" t="s">
+      <c r="L1" s="8"/>
+      <c r="M1" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="N1" s="4"/>
-    </row>
-    <row r="2" spans="1:14" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="N1" s="8"/>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>44</v>
       </c>
@@ -3859,7 +3865,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>48</v>
       </c>
@@ -3900,7 +3906,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>51</v>
       </c>
@@ -3944,7 +3950,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>54</v>
       </c>
@@ -3988,7 +3994,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>57</v>
       </c>
@@ -4027,6 +4033,16 @@
       </c>
       <c r="N10" t="s">
         <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>538</v>
       </c>
     </row>
   </sheetData>
@@ -4050,7 +4066,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="31.375" customWidth="1"/>
     <col min="2" max="2" width="15.75" style="3" customWidth="1"/>
@@ -4077,92 +4093,92 @@
       <c r="F1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4" t="s">
+      <c r="H1" s="8"/>
+      <c r="I1" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4" t="s">
+      <c r="J1" s="8"/>
+      <c r="K1" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="L1" s="4"/>
-      <c r="M1" s="4" t="s">
+      <c r="L1" s="8"/>
+      <c r="M1" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="N1" s="4"/>
-    </row>
-    <row r="2" spans="1:14" s="6" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A2" s="5"/>
-      <c r="B2" s="5" t="s">
+      <c r="N1" s="8"/>
+    </row>
+    <row r="2" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="4"/>
+      <c r="B2" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="I2" s="5"/>
-      <c r="K2" s="5"/>
-      <c r="L2" s="5"/>
-      <c r="M2" s="5"/>
-    </row>
-    <row r="3" spans="1:14" s="6" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A3" s="5"/>
-      <c r="B3" s="5" t="s">
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="K2" s="4"/>
+      <c r="L2" s="4"/>
+      <c r="M2" s="4"/>
+    </row>
+    <row r="3" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="4"/>
+      <c r="B3" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-      <c r="I3" s="5"/>
-      <c r="K3" s="5"/>
-      <c r="L3" s="5"/>
-      <c r="M3" s="5"/>
-    </row>
-    <row r="4" spans="1:14" s="6" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A4" s="5"/>
-      <c r="B4" s="5" t="s">
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="I3" s="4"/>
+      <c r="K3" s="4"/>
+      <c r="L3" s="4"/>
+      <c r="M3" s="4"/>
+    </row>
+    <row r="4" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="4"/>
+      <c r="B4" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-      <c r="I4" s="5"/>
-      <c r="K4" s="5"/>
-      <c r="L4" s="5"/>
-      <c r="M4" s="5"/>
-    </row>
-    <row r="5" spans="1:14" s="6" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A5" s="5"/>
-      <c r="B5" s="5" t="s">
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="K4" s="4"/>
+      <c r="L4" s="4"/>
+      <c r="M4" s="4"/>
+    </row>
+    <row r="5" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="4"/>
+      <c r="B5" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
-      <c r="I5" s="5"/>
-      <c r="K5" s="5"/>
-      <c r="L5" s="5"/>
-      <c r="M5" s="5"/>
-    </row>
-    <row r="6" spans="1:14" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="I5" s="4"/>
+      <c r="K5" s="4"/>
+      <c r="L5" s="4"/>
+      <c r="M5" s="4"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>65</v>
       </c>
@@ -4203,7 +4219,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>68</v>
       </c>
@@ -4244,7 +4260,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>71</v>
       </c>
@@ -4288,7 +4304,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>74</v>
       </c>
@@ -4391,7 +4407,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="27.375" style="3" customWidth="1"/>
     <col min="2" max="2" width="10.625" style="3" customWidth="1"/>
@@ -4412,10 +4428,10 @@
       <c r="C1" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="E1" s="7"/>
+      <c r="E1" s="9"/>
       <c r="F1" s="2" t="s">
         <v>79</v>
       </c>
@@ -4426,7 +4442,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>82</v>
       </c>
@@ -4452,7 +4468,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>87</v>
       </c>
@@ -4478,7 +4494,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>89</v>
       </c>
@@ -4504,7 +4520,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>91</v>
       </c>
@@ -4530,7 +4546,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>93</v>
       </c>
@@ -4556,7 +4572,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>95</v>
       </c>
@@ -4582,7 +4598,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>97</v>
       </c>
@@ -4608,7 +4624,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>99</v>
       </c>
@@ -4634,7 +4650,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>101</v>
       </c>
@@ -4660,7 +4676,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>103</v>
       </c>
@@ -4686,7 +4702,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>105</v>
       </c>
@@ -4712,7 +4728,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>107</v>
       </c>
@@ -4738,7 +4754,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>109</v>
       </c>
@@ -4764,7 +4780,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>111</v>
       </c>
@@ -4790,7 +4806,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>113</v>
       </c>
@@ -4816,7 +4832,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>115</v>
       </c>
@@ -4842,7 +4858,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>117</v>
       </c>
@@ -4868,7 +4884,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
         <v>119</v>
       </c>
@@ -4894,7 +4910,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
         <v>121</v>
       </c>
@@ -4920,7 +4936,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
         <v>123</v>
       </c>
@@ -4946,7 +4962,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
         <v>125</v>
       </c>
@@ -4972,7 +4988,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
         <v>126</v>
       </c>
@@ -4998,7 +5014,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
         <v>127</v>
       </c>
@@ -5024,7 +5040,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
         <v>128</v>
       </c>
@@ -5050,7 +5066,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
         <v>129</v>
       </c>
@@ -5076,7 +5092,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
         <v>130</v>
       </c>
@@ -5102,7 +5118,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
         <v>131</v>
       </c>
@@ -5128,7 +5144,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="29" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
         <v>132</v>
       </c>
@@ -5154,7 +5170,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
         <v>133</v>
       </c>
@@ -5180,7 +5196,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
         <v>134</v>
       </c>
@@ -5206,7 +5222,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="32" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
         <v>135</v>
       </c>
@@ -5232,7 +5248,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="33" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
         <v>136</v>
       </c>
@@ -5258,7 +5274,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="34" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
         <v>137</v>
       </c>
@@ -5284,7 +5300,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="35" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
         <v>138</v>
       </c>
@@ -5310,7 +5326,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="36" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
         <v>139</v>
       </c>
@@ -5336,7 +5352,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="37" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
         <v>140</v>
       </c>
@@ -5362,7 +5378,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="38" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
         <v>141</v>
       </c>
@@ -5388,7 +5404,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="39" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
         <v>142</v>
       </c>
@@ -5414,7 +5430,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="40" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" s="3" t="s">
         <v>143</v>
       </c>
@@ -5440,7 +5456,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="41" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" s="3" t="s">
         <v>144</v>
       </c>
@@ -5466,7 +5482,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="42" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" s="3" t="s">
         <v>146</v>
       </c>
@@ -5492,7 +5508,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="43" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" s="3" t="s">
         <v>148</v>
       </c>
@@ -5518,7 +5534,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="44" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44" s="3" t="s">
         <v>150</v>
       </c>
@@ -5544,7 +5560,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="45" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A45" s="3" t="s">
         <v>152</v>
       </c>
@@ -5570,7 +5586,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="46" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A46" s="3" t="s">
         <v>154</v>
       </c>
@@ -5596,7 +5612,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="47" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A47" s="3" t="s">
         <v>156</v>
       </c>
@@ -5622,7 +5638,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="48" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48" s="3" t="s">
         <v>158</v>
       </c>
@@ -5648,7 +5664,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="49" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49" s="3" t="s">
         <v>160</v>
       </c>
@@ -5674,7 +5690,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="50" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A50" s="3" t="s">
         <v>162</v>
       </c>
@@ -5700,7 +5716,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="51" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A51" s="3" t="s">
         <v>164</v>
       </c>
@@ -5726,7 +5742,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="52" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A52" s="3" t="s">
         <v>166</v>
       </c>
@@ -5752,7 +5768,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="53" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A53" s="3" t="s">
         <v>168</v>
       </c>
@@ -5778,7 +5794,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="54" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A54" s="3" t="s">
         <v>170</v>
       </c>
@@ -5804,7 +5820,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="55" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A55" s="3" t="s">
         <v>172</v>
       </c>
@@ -5830,7 +5846,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="56" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A56" s="3" t="s">
         <v>174</v>
       </c>
@@ -5856,7 +5872,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="57" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A57" s="3" t="s">
         <v>176</v>
       </c>
@@ -5882,7 +5898,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="58" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A58" s="3" t="s">
         <v>178</v>
       </c>
@@ -5908,7 +5924,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="59" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A59" s="3" t="s">
         <v>180</v>
       </c>
@@ -5934,7 +5950,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="60" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A60" s="3" t="s">
         <v>182</v>
       </c>
@@ -5960,7 +5976,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="61" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A61" s="3" t="s">
         <v>184</v>
       </c>
@@ -5986,7 +6002,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="62" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A62" s="3" t="s">
         <v>186</v>
       </c>
@@ -6012,7 +6028,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="63" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A63" s="3" t="s">
         <v>188</v>
       </c>
@@ -6038,7 +6054,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="64" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A64" s="3" t="s">
         <v>190</v>
       </c>
@@ -6064,7 +6080,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="65" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A65" s="3" t="s">
         <v>192</v>
       </c>
@@ -6090,7 +6106,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="66" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A66" s="3" t="s">
         <v>194</v>
       </c>
@@ -6116,7 +6132,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="67" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A67" s="3" t="s">
         <v>196</v>
       </c>
@@ -6142,7 +6158,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="68" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A68" s="3" t="s">
         <v>198</v>
       </c>
@@ -6168,7 +6184,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="69" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A69" s="3" t="s">
         <v>200</v>
       </c>
@@ -6194,7 +6210,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="70" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A70" s="3" t="s">
         <v>202</v>
       </c>
@@ -6220,7 +6236,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="71" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A71" s="3" t="s">
         <v>204</v>
       </c>
@@ -6246,7 +6262,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="72" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A72" s="3" t="s">
         <v>206</v>
       </c>
@@ -6272,7 +6288,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="73" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A73" s="3" t="s">
         <v>207</v>
       </c>
@@ -6298,7 +6314,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="74" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A74" s="3" t="s">
         <v>208</v>
       </c>
@@ -6324,7 +6340,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="75" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A75" s="3" t="s">
         <v>209</v>
       </c>
@@ -6350,7 +6366,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="76" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A76" s="3" t="s">
         <v>210</v>
       </c>
@@ -6376,7 +6392,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="77" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A77" s="3" t="s">
         <v>211</v>
       </c>
@@ -6402,7 +6418,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="78" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A78" s="3" t="s">
         <v>212</v>
       </c>
@@ -6428,7 +6444,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="79" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A79" s="3" t="s">
         <v>213</v>
       </c>
@@ -6454,7 +6470,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="80" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A80" s="3" t="s">
         <v>214</v>
       </c>
@@ -6480,7 +6496,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="81" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A81" s="3" t="s">
         <v>215</v>
       </c>
@@ -6506,7 +6522,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="82" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A82" s="3" t="s">
         <v>216</v>
       </c>
@@ -6532,7 +6548,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="83" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A83" s="3" t="s">
         <v>217</v>
       </c>
@@ -6558,7 +6574,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="84" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A84" s="3" t="s">
         <v>218</v>
       </c>
@@ -6584,7 +6600,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="85" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A85" s="3" t="s">
         <v>219</v>
       </c>
@@ -6610,7 +6626,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="86" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A86" s="3" t="s">
         <v>220</v>
       </c>
@@ -6636,7 +6652,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="87" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A87" s="3" t="s">
         <v>221</v>
       </c>
@@ -6662,7 +6678,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="88" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A88" s="3" t="s">
         <v>222</v>
       </c>
@@ -6688,7 +6704,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="89" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A89" s="3" t="s">
         <v>223</v>
       </c>
@@ -6714,7 +6730,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="90" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A90" s="3" t="s">
         <v>224</v>
       </c>
@@ -6740,7 +6756,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="91" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A91" s="3" t="s">
         <v>225</v>
       </c>
@@ -6766,7 +6782,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="92" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A92" s="3" t="s">
         <v>226</v>
       </c>
@@ -6792,7 +6808,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="93" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A93" s="3" t="s">
         <v>227</v>
       </c>
@@ -6818,7 +6834,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="94" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A94" s="3" t="s">
         <v>228</v>
       </c>
@@ -6844,7 +6860,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="95" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A95" s="3" t="s">
         <v>229</v>
       </c>
@@ -6870,7 +6886,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="96" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A96" s="3" t="s">
         <v>230</v>
       </c>
@@ -6896,7 +6912,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="97" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A97" s="3" t="s">
         <v>231</v>
       </c>
@@ -6922,7 +6938,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="98" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A98" s="3" t="s">
         <v>232</v>
       </c>
@@ -6948,7 +6964,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="99" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A99" s="3" t="s">
         <v>233</v>
       </c>
@@ -6974,7 +6990,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="100" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A100" s="3" t="s">
         <v>234</v>
       </c>
@@ -7000,7 +7016,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="101" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A101" s="3" t="s">
         <v>235</v>
       </c>
@@ -7026,7 +7042,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="102" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A102" s="3" t="s">
         <v>236</v>
       </c>
@@ -7052,7 +7068,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="103" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A103" s="3" t="s">
         <v>237</v>
       </c>
@@ -7078,7 +7094,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="104" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A104" s="3" t="s">
         <v>238</v>
       </c>
@@ -7104,7 +7120,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="105" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A105" s="3" t="s">
         <v>239</v>
       </c>
@@ -7130,7 +7146,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="106" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A106" s="3" t="s">
         <v>240</v>
       </c>
@@ -7156,7 +7172,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="107" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A107" s="3" t="s">
         <v>241</v>
       </c>
@@ -7182,7 +7198,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="108" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A108" s="3" t="s">
         <v>242</v>
       </c>
@@ -7208,7 +7224,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="109" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A109" s="3" t="s">
         <v>243</v>
       </c>
@@ -7234,7 +7250,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="110" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A110" s="3" t="s">
         <v>244</v>
       </c>
@@ -7260,7 +7276,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="111" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A111" s="3" t="s">
         <v>245</v>
       </c>
@@ -7286,7 +7302,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="112" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A112" s="3" t="s">
         <v>246</v>
       </c>
@@ -7312,7 +7328,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="113" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A113" s="3" t="s">
         <v>247</v>
       </c>
@@ -7338,7 +7354,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="114" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A114" s="3" t="s">
         <v>248</v>
       </c>
@@ -7364,7 +7380,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="115" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A115" s="3" t="s">
         <v>249</v>
       </c>
@@ -7390,7 +7406,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="116" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A116" s="3" t="s">
         <v>250</v>
       </c>
@@ -7416,7 +7432,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="117" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A117" s="3" t="s">
         <v>251</v>
       </c>
@@ -7442,7 +7458,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="118" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A118" s="3" t="s">
         <v>252</v>
       </c>
@@ -7468,7 +7484,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="119" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A119" s="3" t="s">
         <v>253</v>
       </c>
@@ -7494,7 +7510,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="120" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A120" s="3" t="s">
         <v>254</v>
       </c>
@@ -7520,7 +7536,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="121" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A121" s="3" t="s">
         <v>255</v>
       </c>
@@ -7546,7 +7562,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="122" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A122" s="3" t="s">
         <v>256</v>
       </c>
@@ -7572,7 +7588,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="123" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A123" s="3" t="s">
         <v>257</v>
       </c>
@@ -7598,7 +7614,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="124" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A124" s="3" t="s">
         <v>258</v>
       </c>
@@ -7624,7 +7640,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="125" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A125" s="3" t="s">
         <v>259</v>
       </c>
@@ -7650,7 +7666,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="126" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A126" s="3" t="s">
         <v>260</v>
       </c>
@@ -7676,7 +7692,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="127" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A127" s="3" t="s">
         <v>261</v>
       </c>
@@ -7702,7 +7718,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="128" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A128" s="3" t="s">
         <v>262</v>
       </c>
@@ -7728,7 +7744,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="129" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A129" s="3" t="s">
         <v>263</v>
       </c>
@@ -7754,7 +7770,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="130" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A130" s="3" t="s">
         <v>264</v>
       </c>
@@ -7780,7 +7796,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="131" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A131" s="3" t="s">
         <v>265</v>
       </c>
@@ -7806,7 +7822,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="132" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A132" s="3" t="s">
         <v>266</v>
       </c>
@@ -7832,7 +7848,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="133" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A133" s="3" t="s">
         <v>267</v>
       </c>
@@ -7858,7 +7874,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="134" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A134" s="3" t="s">
         <v>268</v>
       </c>
@@ -7884,7 +7900,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="135" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A135" s="3" t="s">
         <v>269</v>
       </c>
@@ -7910,7 +7926,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="136" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A136" s="3" t="s">
         <v>270</v>
       </c>
@@ -7936,7 +7952,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="137" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A137" s="3" t="s">
         <v>271</v>
       </c>
@@ -7962,7 +7978,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="138" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A138" s="3" t="s">
         <v>272</v>
       </c>
@@ -7988,7 +8004,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="139" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A139" s="3" t="s">
         <v>273</v>
       </c>
@@ -8014,7 +8030,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="140" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A140" s="3" t="s">
         <v>274</v>
       </c>
@@ -8040,7 +8056,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="141" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A141" s="3" t="s">
         <v>276</v>
       </c>
@@ -8066,7 +8082,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="142" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A142" s="3" t="s">
         <v>277</v>
       </c>
@@ -8092,7 +8108,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="143" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A143" s="3" t="s">
         <v>278</v>
       </c>
@@ -8118,7 +8134,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="144" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A144" s="3" t="s">
         <v>279</v>
       </c>
@@ -8144,7 +8160,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="145" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A145" s="3" t="s">
         <v>280</v>
       </c>
@@ -8170,7 +8186,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="146" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A146" s="3" t="s">
         <v>281</v>
       </c>
@@ -8196,7 +8212,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="147" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A147" s="3" t="s">
         <v>282</v>
       </c>
@@ -8222,7 +8238,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="148" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A148" s="3" t="s">
         <v>283</v>
       </c>
@@ -8248,7 +8264,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="149" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A149" s="3" t="s">
         <v>284</v>
       </c>
@@ -8274,7 +8290,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="150" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A150" s="3" t="s">
         <v>285</v>
       </c>
@@ -8300,7 +8316,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="151" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A151" s="3" t="s">
         <v>286</v>
       </c>
@@ -8326,7 +8342,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="152" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A152" s="3" t="s">
         <v>287</v>
       </c>
@@ -8352,7 +8368,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="153" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A153" s="3" t="s">
         <v>288</v>
       </c>
@@ -8378,7 +8394,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="154" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A154" s="3" t="s">
         <v>289</v>
       </c>
@@ -8404,7 +8420,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="155" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A155" s="3" t="s">
         <v>290</v>
       </c>
@@ -8430,7 +8446,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="156" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A156" s="3" t="s">
         <v>291</v>
       </c>
@@ -8456,7 +8472,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="157" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A157" s="3" t="s">
         <v>292</v>
       </c>
@@ -8482,7 +8498,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="158" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A158" s="3" t="s">
         <v>293</v>
       </c>
@@ -8508,7 +8524,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="159" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A159" s="3" t="s">
         <v>294</v>
       </c>
@@ -8534,7 +8550,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="160" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A160" s="3" t="s">
         <v>295</v>
       </c>
@@ -8560,7 +8576,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="161" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A161" s="3" t="s">
         <v>296</v>
       </c>
@@ -8586,7 +8602,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="162" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A162" s="3" t="s">
         <v>297</v>
       </c>
@@ -8612,7 +8628,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="163" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A163" s="3" t="s">
         <v>298</v>
       </c>
@@ -8638,7 +8654,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="164" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A164" s="3" t="s">
         <v>299</v>
       </c>
@@ -8664,7 +8680,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="165" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A165" s="3" t="s">
         <v>300</v>
       </c>
@@ -8690,7 +8706,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="166" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A166" s="3" t="s">
         <v>301</v>
       </c>
@@ -8716,7 +8732,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="167" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A167" s="3" t="s">
         <v>302</v>
       </c>
@@ -8742,7 +8758,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="168" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A168" s="3" t="s">
         <v>303</v>
       </c>
@@ -8768,7 +8784,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="169" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A169" s="3" t="s">
         <v>304</v>
       </c>
@@ -8794,7 +8810,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="170" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A170" s="3" t="s">
         <v>305</v>
       </c>
@@ -8820,7 +8836,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="171" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A171" s="3" t="s">
         <v>306</v>
       </c>
@@ -8846,7 +8862,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="172" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A172" s="3" t="s">
         <v>307</v>
       </c>
@@ -8872,7 +8888,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="173" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A173" s="3" t="s">
         <v>308</v>
       </c>
@@ -8898,7 +8914,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="174" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A174" s="3" t="s">
         <v>309</v>
       </c>
@@ -8924,7 +8940,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="175" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A175" s="3" t="s">
         <v>310</v>
       </c>
@@ -8950,7 +8966,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="176" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A176" s="3" t="s">
         <v>311</v>
       </c>
@@ -8976,7 +8992,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="177" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A177" s="3" t="s">
         <v>312</v>
       </c>
@@ -9002,7 +9018,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="178" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A178" s="3" t="s">
         <v>313</v>
       </c>
@@ -9028,7 +9044,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="179" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A179" s="3" t="s">
         <v>314</v>
       </c>
@@ -9054,7 +9070,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="180" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A180" s="3" t="s">
         <v>315</v>
       </c>
@@ -9080,7 +9096,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="181" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A181" s="3" t="s">
         <v>316</v>
       </c>
@@ -9106,7 +9122,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="182" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A182" s="3" t="s">
         <v>317</v>
       </c>
@@ -9132,7 +9148,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="183" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A183" s="3" t="s">
         <v>318</v>
       </c>
@@ -9158,7 +9174,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="184" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A184" s="3" t="s">
         <v>319</v>
       </c>
@@ -9184,7 +9200,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="185" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A185" s="3" t="s">
         <v>320</v>
       </c>
@@ -9210,7 +9226,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="186" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A186" s="3" t="s">
         <v>321</v>
       </c>
@@ -9236,7 +9252,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="187" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A187" s="3" t="s">
         <v>322</v>
       </c>
@@ -9262,7 +9278,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="188" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A188" s="3" t="s">
         <v>323</v>
       </c>
@@ -9288,7 +9304,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="189" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A189" s="3" t="s">
         <v>324</v>
       </c>
@@ -9314,7 +9330,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="190" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A190" s="3" t="s">
         <v>325</v>
       </c>
@@ -9340,7 +9356,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="191" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A191" s="3" t="s">
         <v>326</v>
       </c>
@@ -9366,7 +9382,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="192" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A192" s="3" t="s">
         <v>327</v>
       </c>
@@ -9392,7 +9408,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="193" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A193" s="3" t="s">
         <v>328</v>
       </c>
@@ -9418,7 +9434,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="194" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A194" s="3" t="s">
         <v>329</v>
       </c>
@@ -9444,7 +9460,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="195" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A195" s="3" t="s">
         <v>330</v>
       </c>
@@ -9470,7 +9486,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="196" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A196" s="3" t="s">
         <v>331</v>
       </c>
@@ -9496,7 +9512,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="197" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A197" s="3" t="s">
         <v>332</v>
       </c>
@@ -9522,7 +9538,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="198" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A198" s="3" t="s">
         <v>333</v>
       </c>
@@ -9548,7 +9564,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="199" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A199" s="3" t="s">
         <v>334</v>
       </c>
@@ -9574,7 +9590,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="200" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A200" s="3" t="s">
         <v>335</v>
       </c>
@@ -9600,7 +9616,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="201" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A201" s="3" t="s">
         <v>336</v>
       </c>
@@ -9626,7 +9642,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="202" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A202" s="3" t="s">
         <v>337</v>
       </c>
@@ -9652,7 +9668,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="203" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A203" s="3" t="s">
         <v>338</v>
       </c>
@@ -9678,7 +9694,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="204" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A204" s="3" t="s">
         <v>339</v>
       </c>
@@ -9704,7 +9720,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="205" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A205" s="3" t="s">
         <v>340</v>
       </c>
@@ -9730,7 +9746,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="206" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A206" s="3" t="s">
         <v>341</v>
       </c>
@@ -9756,7 +9772,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="207" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A207" s="3" t="s">
         <v>342</v>
       </c>
@@ -9782,7 +9798,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="208" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A208" s="3" t="s">
         <v>343</v>
       </c>
@@ -9808,7 +9824,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="209" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A209" s="3" t="s">
         <v>344</v>
       </c>
@@ -9834,7 +9850,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="210" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A210" s="3" t="s">
         <v>345</v>
       </c>
@@ -9860,7 +9876,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="211" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A211" s="3" t="s">
         <v>346</v>
       </c>
@@ -9886,7 +9902,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="212" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A212" s="3" t="s">
         <v>347</v>
       </c>
@@ -9912,7 +9928,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="213" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A213" s="3" t="s">
         <v>348</v>
       </c>
@@ -9938,7 +9954,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="214" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A214" s="3" t="s">
         <v>349</v>
       </c>
@@ -9964,7 +9980,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="215" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A215" s="3" t="s">
         <v>350</v>
       </c>
@@ -9990,7 +10006,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="216" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A216" s="3" t="s">
         <v>351</v>
       </c>
@@ -10016,7 +10032,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="217" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A217" s="3" t="s">
         <v>352</v>
       </c>
@@ -10042,7 +10058,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="218" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A218" s="3" t="s">
         <v>353</v>
       </c>
@@ -10068,7 +10084,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="219" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A219" s="3" t="s">
         <v>354</v>
       </c>
@@ -10094,7 +10110,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="220" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A220" s="3" t="s">
         <v>355</v>
       </c>
@@ -10120,7 +10136,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="221" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A221" s="3" t="s">
         <v>356</v>
       </c>
@@ -10146,7 +10162,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="222" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A222" s="3" t="s">
         <v>357</v>
       </c>
@@ -10172,7 +10188,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="223" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A223" s="3" t="s">
         <v>358</v>
       </c>
@@ -10198,7 +10214,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="224" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="224" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A224" s="3" t="s">
         <v>359</v>
       </c>
@@ -10224,7 +10240,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="225" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A225" s="3" t="s">
         <v>360</v>
       </c>
@@ -10250,7 +10266,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="226" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A226" s="3" t="s">
         <v>361</v>
       </c>
@@ -10276,7 +10292,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="227" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A227" s="3" t="s">
         <v>362</v>
       </c>
@@ -10302,7 +10318,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="228" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A228" s="3" t="s">
         <v>363</v>
       </c>
@@ -10328,7 +10344,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="229" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A229" s="3" t="s">
         <v>364</v>
       </c>
@@ -10354,7 +10370,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="230" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A230" s="3" t="s">
         <v>365</v>
       </c>
@@ -10380,7 +10396,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="231" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A231" s="3" t="s">
         <v>366</v>
       </c>
@@ -10406,7 +10422,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="232" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A232" s="3" t="s">
         <v>367</v>
       </c>
@@ -10432,7 +10448,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="233" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A233" s="3" t="s">
         <v>368</v>
       </c>
@@ -10458,7 +10474,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="234" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A234" s="3" t="s">
         <v>369</v>
       </c>
@@ -10484,7 +10500,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="235" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A235" s="3" t="s">
         <v>370</v>
       </c>
@@ -10510,7 +10526,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="236" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A236" s="3" t="s">
         <v>371</v>
       </c>
@@ -10536,7 +10552,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="237" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A237" s="3" t="s">
         <v>372</v>
       </c>
@@ -10562,7 +10578,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="238" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A238" s="3" t="s">
         <v>373</v>
       </c>
@@ -10588,7 +10604,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="239" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="239" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A239" s="3" t="s">
         <v>374</v>
       </c>
@@ -10614,7 +10630,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="240" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="240" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A240" s="3" t="s">
         <v>375</v>
       </c>
@@ -10640,7 +10656,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="241" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A241" s="3" t="s">
         <v>376</v>
       </c>
@@ -10666,7 +10682,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="242" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="242" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A242" s="3" t="s">
         <v>377</v>
       </c>
@@ -10692,7 +10708,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="243" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A243" s="3" t="s">
         <v>378</v>
       </c>
@@ -10718,7 +10734,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="244" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="244" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A244" s="3" t="s">
         <v>379</v>
       </c>
@@ -10744,7 +10760,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="245" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="245" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A245" s="3" t="s">
         <v>380</v>
       </c>
@@ -10770,7 +10786,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="246" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="246" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A246" s="3" t="s">
         <v>381</v>
       </c>
@@ -10796,7 +10812,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="247" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="247" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A247" s="3" t="s">
         <v>382</v>
       </c>
@@ -10822,7 +10838,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="248" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="248" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A248" s="3" t="s">
         <v>383</v>
       </c>
@@ -10848,7 +10864,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="249" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="249" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A249" s="3" t="s">
         <v>384</v>
       </c>
@@ -10874,7 +10890,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="250" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="250" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A250" s="3" t="s">
         <v>385</v>
       </c>
@@ -10900,7 +10916,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="251" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="251" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A251" s="3" t="s">
         <v>386</v>
       </c>
@@ -10926,7 +10942,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="252" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="252" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A252" s="3" t="s">
         <v>387</v>
       </c>
@@ -10952,7 +10968,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="253" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="253" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A253" s="3" t="s">
         <v>388</v>
       </c>
@@ -10978,7 +10994,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="254" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="254" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A254" s="3" t="s">
         <v>389</v>
       </c>
@@ -11004,7 +11020,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="255" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="255" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A255" s="3" t="s">
         <v>390</v>
       </c>
@@ -11030,7 +11046,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="256" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="256" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A256" s="3" t="s">
         <v>391</v>
       </c>
@@ -11056,7 +11072,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="257" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="257" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A257" s="3" t="s">
         <v>392</v>
       </c>
@@ -11082,7 +11098,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="258" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="258" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A258" s="3" t="s">
         <v>393</v>
       </c>
@@ -11108,7 +11124,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="259" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="259" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A259" s="3" t="s">
         <v>394</v>
       </c>
@@ -11134,7 +11150,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="260" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="260" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A260" s="3" t="s">
         <v>395</v>
       </c>
@@ -11160,7 +11176,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="261" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="261" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A261" s="3" t="s">
         <v>396</v>
       </c>
@@ -11186,7 +11202,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="262" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="262" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A262" s="3" t="s">
         <v>397</v>
       </c>
@@ -11212,7 +11228,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="263" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="263" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A263" s="3" t="s">
         <v>398</v>
       </c>
@@ -11238,7 +11254,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="264" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="264" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A264" s="3" t="s">
         <v>399</v>
       </c>
@@ -11264,7 +11280,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="265" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="265" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A265" s="3" t="s">
         <v>400</v>
       </c>
@@ -11290,7 +11306,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="266" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="266" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A266" s="3" t="s">
         <v>401</v>
       </c>
@@ -11316,7 +11332,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="267" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="267" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A267" s="3" t="s">
         <v>402</v>
       </c>
@@ -11342,7 +11358,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="268" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="268" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A268" s="3" t="s">
         <v>403</v>
       </c>
@@ -11368,7 +11384,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="269" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="269" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A269" s="3" t="s">
         <v>404</v>
       </c>
@@ -11394,7 +11410,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="270" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="270" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A270" s="3" t="s">
         <v>405</v>
       </c>
@@ -11420,7 +11436,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="271" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="271" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A271" s="3" t="s">
         <v>406</v>
       </c>
@@ -11446,7 +11462,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="272" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="272" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A272" s="3" t="s">
         <v>407</v>
       </c>
@@ -11472,7 +11488,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="273" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="273" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A273" s="3" t="s">
         <v>408</v>
       </c>
@@ -11498,7 +11514,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="274" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="274" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A274" s="3" t="s">
         <v>409</v>
       </c>
@@ -11524,7 +11540,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="275" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="275" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A275" s="3" t="s">
         <v>410</v>
       </c>
@@ -11550,7 +11566,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="276" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="276" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A276" s="3" t="s">
         <v>411</v>
       </c>
@@ -11576,7 +11592,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="277" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="277" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A277" s="3" t="s">
         <v>412</v>
       </c>

</xml_diff>